<commit_message>
Added registers and test benches
</commit_message>
<xml_diff>
--- a/Processor.xlsx
+++ b/Processor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="266">
   <si>
     <t>RA &lt;== T</t>
   </si>
@@ -1278,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="73" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1924,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2203,12 +2203,8 @@
       <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="M15" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="N15" s="10">
-        <v>1000</v>
-      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -2453,9 +2449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AB81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2340" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2340" topLeftCell="A61" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removed unwanted Abus and Ram wires, tested NOP in ALU
</commit_message>
<xml_diff>
--- a/Processor.xlsx
+++ b/Processor.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="265">
   <si>
     <t>RA &lt;== T</t>
   </si>
@@ -679,9 +680,6 @@
   </si>
   <si>
     <t>0110</t>
-  </si>
-  <si>
-    <t>0111</t>
   </si>
   <si>
     <t>DR &lt;== AC, write</t>
@@ -1278,7 +1276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="95" zoomScaleNormal="73" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1924,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1958,10 +1956,10 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
         <v>143</v>
@@ -1996,15 +1994,15 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
       <c r="Q5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
@@ -2038,18 +2036,18 @@
         <v>153</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>211</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E8" t="s">
         <v>134</v>
@@ -2067,7 +2065,7 @@
         <v>207</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
@@ -2078,13 +2076,13 @@
         <v>155</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>208</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
@@ -2098,13 +2096,13 @@
         <v>164</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q10" s="9" t="s">
         <v>209</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
@@ -2127,13 +2125,13 @@
         <v>165</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q11" s="9" t="s">
         <v>210</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
@@ -2150,13 +2148,13 @@
         <v>166</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q12" s="15">
         <v>101</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
@@ -2170,13 +2168,13 @@
         <v>161</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q13" s="15">
         <v>111</v>
       </c>
       <c r="R13" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
@@ -2186,12 +2184,8 @@
       <c r="B14" t="s">
         <v>132</v>
       </c>
-      <c r="M14" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>219</v>
-      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -2258,7 +2252,7 @@
         <v>138</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N19" s="10">
         <v>1111</v>
@@ -2369,15 +2363,15 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
@@ -2388,7 +2382,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B33" t="s">
         <v>169</v>
@@ -2449,9 +2443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AB81"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2340" topLeftCell="A61" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2470,19 +2464,19 @@
   <sheetData>
     <row r="3" spans="1:28" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
@@ -2495,22 +2489,22 @@
       <c r="S3" s="18"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="V3" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="W3" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="Y3" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>244</v>
       </c>
       <c r="AA3" s="13" t="s">
         <v>173</v>
@@ -3528,7 +3522,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E20" s="14">
         <v>13</v>
@@ -3688,7 +3682,7 @@
         <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E23" s="14">
         <v>15</v>
@@ -3848,7 +3842,7 @@
         <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E26" s="14">
         <v>17</v>
@@ -4788,7 +4782,7 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E42" s="14">
         <v>29</v>
@@ -5008,7 +5002,7 @@
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E46" s="14">
         <v>32</v>
@@ -5227,7 +5221,7 @@
     </row>
     <row r="50" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E50" s="14">
         <v>35</v>
@@ -5302,7 +5296,7 @@
     </row>
     <row r="52" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E52" s="14">
         <v>36</v>
@@ -5374,7 +5368,7 @@
     </row>
     <row r="53" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E53" s="14">
         <v>37</v>
@@ -5446,7 +5440,7 @@
     </row>
     <row r="54" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E54" s="14">
         <v>38</v>
@@ -6473,7 +6467,7 @@
     </row>
     <row r="74" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E74" s="14">
         <v>52</v>
@@ -6546,7 +6540,7 @@
     </row>
     <row r="75" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E75" s="7">
         <v>53</v>
@@ -6621,7 +6615,7 @@
     </row>
     <row r="77" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E77" s="7">
         <v>54</v>
@@ -6696,7 +6690,7 @@
     </row>
     <row r="79" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E79" s="7">
         <v>55</v>

</xml_diff>

<commit_message>
Completed one core, added end operation
</commit_message>
<xml_diff>
--- a/Processor.xlsx
+++ b/Processor.xlsx
@@ -4,16 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="268">
   <si>
     <t>RA &lt;== T</t>
   </si>
@@ -430,15 +429,6 @@
     <t>M &lt;== DR</t>
   </si>
   <si>
-    <t>ADD1</t>
-  </si>
-  <si>
-    <t>ADD2</t>
-  </si>
-  <si>
-    <t>ADD3</t>
-  </si>
-  <si>
     <t>RA &lt;= RA + 1</t>
   </si>
   <si>
@@ -818,6 +808,24 @@
   </si>
   <si>
     <t>AC pass</t>
+  </si>
+  <si>
+    <t>EX - 1</t>
+  </si>
+  <si>
+    <t>JPNZ</t>
+  </si>
+  <si>
+    <t>if z==0 =&gt; JUMP</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>ENDOP</t>
   </si>
 </sst>
 </file>
@@ -900,7 +908,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -938,12 +946,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -987,11 +1013,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1274,616 +1328,1088 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W49"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="95" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" customWidth="1"/>
-    <col min="7" max="7" width="3.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="19.77734375" customWidth="1"/>
-    <col min="17" max="17" width="8.6640625" customWidth="1"/>
+    <col min="3" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="3.88671875" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.77734375" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="H1" t="s">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="I1" s="16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="P2" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Q2" t="s">
         <v>115</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="D3" s="14">
+        <v>4</v>
+      </c>
+      <c r="E3" s="23" t="str">
+        <f t="shared" ref="E3:E4" si="0">TEXT(DEC2BIN(D3),"000000")</f>
+        <v>000100</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>48</v>
       </c>
-      <c r="M3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="D4" s="14">
+        <v>36</v>
+      </c>
+      <c r="E4" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>100100</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>49</v>
       </c>
-      <c r="M4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="D5" s="14">
+        <v>4</v>
+      </c>
+      <c r="E5" s="23" t="str">
+        <f t="shared" ref="E5:E6" si="1">TEXT(DEC2BIN(D5),"000000")</f>
+        <v>000100</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>50</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="D6" s="14">
+        <v>37</v>
+      </c>
+      <c r="E6" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>100101</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="2:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H7" s="3" t="s">
+    <row r="7" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>42</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="X7" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="D8" s="14">
+        <v>12</v>
+      </c>
+      <c r="E8" s="23" t="str">
+        <f t="shared" ref="E8:E10" si="2">TEXT(DEC2BIN(D8),"000000")</f>
+        <v>001100</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>44</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="D9" s="14">
+        <v>14</v>
+      </c>
+      <c r="E9" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>001110</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>46</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="D10" s="14">
+        <v>16</v>
+      </c>
+      <c r="E10" s="23" t="str">
+        <f t="shared" si="2"/>
+        <v>010000</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="H11" s="3" t="s">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="I11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>38</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>66</v>
       </c>
       <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="D12" s="14">
+        <v>18</v>
+      </c>
+      <c r="E12" s="23" t="str">
+        <f t="shared" ref="E12:E19" si="3">TEXT(DEC2BIN(D12),"000000")</f>
+        <v>010010</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>39</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="P12" s="18">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>1</v>
+      </c>
+      <c r="R12" s="19"/>
+      <c r="S12" s="20"/>
+      <c r="U12" s="18">
+        <v>34</v>
+      </c>
+      <c r="V12" s="21">
+        <v>54</v>
+      </c>
+      <c r="W12" s="19"/>
+      <c r="X12" s="20"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="D13" s="14">
+        <v>38</v>
+      </c>
+      <c r="E13" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>100110</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>43</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="P13" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>4</v>
+      </c>
+      <c r="R13" s="19"/>
+      <c r="S13" s="20"/>
+      <c r="U13" s="18">
+        <v>55</v>
+      </c>
+      <c r="V13" s="21">
+        <v>67</v>
+      </c>
+      <c r="W13" s="19"/>
+      <c r="X13" s="20"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="D14" s="14">
+        <v>21</v>
+      </c>
+      <c r="E14" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>010101</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="O14" s="20"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="20"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="D15" s="14">
+        <v>51</v>
+      </c>
+      <c r="E15" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>110011</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>51</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="D16" s="14">
+        <v>38</v>
+      </c>
+      <c r="E16" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>100110</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>52</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+    </row>
+    <row r="17" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="D17" s="14">
+        <v>24</v>
+      </c>
+      <c r="E17" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>011000</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>45</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+    </row>
+    <row r="18" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="D18" s="14">
+        <v>41</v>
+      </c>
+      <c r="E18" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>101001</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+    </row>
+    <row r="19" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>55</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="D19" s="14">
+        <v>33</v>
+      </c>
+      <c r="E19" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>100001</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>53</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="H20" s="3" t="s">
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+    </row>
+    <row r="20" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="I20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>54</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="D21" s="14">
+        <v>43</v>
+      </c>
+      <c r="E21" s="23" t="str">
+        <f t="shared" ref="E21:E22" si="4">TEXT(DEC2BIN(D21),"000000")</f>
+        <v>101011</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>55</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="D22" s="14">
+        <v>44</v>
+      </c>
+      <c r="E22" s="23" t="str">
+        <f t="shared" si="4"/>
+        <v>101100</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="H23" s="3" t="s">
+    <row r="23" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="I23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>121</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="D24" s="14">
+        <v>4</v>
+      </c>
+      <c r="E24" s="23" t="str">
+        <f t="shared" ref="E24:E28" si="5">TEXT(DEC2BIN(D24),"000000")</f>
+        <v>000100</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>120</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>77</v>
       </c>
-      <c r="K25" t="s">
+      <c r="D25" s="14">
+        <v>48</v>
+      </c>
+      <c r="E25" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v>110000</v>
+      </c>
+      <c r="L25" t="s">
         <v>47</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="27" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="D26" s="14">
+        <v>8</v>
+      </c>
+      <c r="E26" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v>001000</v>
+      </c>
+    </row>
+    <row r="27" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>68</v>
       </c>
-      <c r="K27" t="s">
+      <c r="D27" s="14">
+        <v>46</v>
+      </c>
+      <c r="E27" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v>101110</v>
+      </c>
+      <c r="L27" t="s">
         <v>60</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>76</v>
       </c>
-      <c r="K28" t="s">
+      <c r="D28" s="14">
+        <v>52</v>
+      </c>
+      <c r="E28" s="23" t="str">
+        <f t="shared" si="5"/>
+        <v>110100</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="L28" t="s">
         <v>61</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>64</v>
       </c>
-      <c r="V28" s="4"/>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="K29" t="s">
+      <c r="W28" s="4"/>
+    </row>
+    <row r="29" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
         <v>62</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:24" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="D30" s="14">
+        <v>42</v>
+      </c>
+      <c r="E30" s="23" t="str">
+        <f t="shared" ref="E30:E31" si="6">TEXT(DEC2BIN(D30),"000000")</f>
+        <v>101010</v>
+      </c>
+    </row>
+    <row r="31" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="C31" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K31" t="s">
+      <c r="D31" s="28">
+        <v>43</v>
+      </c>
+      <c r="E31" s="23" t="str">
+        <f t="shared" si="6"/>
+        <v>101011</v>
+      </c>
+      <c r="F31">
+        <v>50</v>
+      </c>
+      <c r="G31" t="str">
+        <f>"8'h"&amp;DEC2HEX(F31, 2)</f>
+        <v>8'h32</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31" t="s">
         <v>67</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="K32" t="s">
+    <row r="32" spans="3:24" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>51</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" ref="G32:G44" si="7">"8'h"&amp;DEC2HEX(F32, 2)</f>
+        <v>8'h33</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" t="s">
         <v>68</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>117</v>
       </c>
-      <c r="K33" t="s">
+      <c r="D33" s="23">
+        <v>55</v>
+      </c>
+      <c r="E33" s="23" t="str">
+        <f t="shared" ref="E33:E34" si="8">TEXT(DEC2BIN(D33),"000000")</f>
+        <v>110111</v>
+      </c>
+      <c r="F33">
+        <v>52</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h34</v>
+      </c>
+      <c r="I33" s="3">
+        <v>2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>265</v>
+      </c>
+      <c r="L33" t="s">
         <v>69</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="K35" t="s">
+      <c r="D34" s="14">
+        <v>8</v>
+      </c>
+      <c r="E34" s="23" t="str">
+        <f t="shared" si="8"/>
+        <v>001000</v>
+      </c>
+      <c r="F34">
+        <v>53</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h35</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>54</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h36</v>
+      </c>
+      <c r="I35" s="3">
+        <v>2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>29</v>
+      </c>
+      <c r="L35" t="s">
         <v>77</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>82</v>
       </c>
-      <c r="K36" t="s">
+      <c r="D36" s="14">
+        <v>4</v>
+      </c>
+      <c r="E36" s="23" t="str">
+        <f t="shared" ref="E36:E39" si="9">TEXT(DEC2BIN(D36),"000000")</f>
+        <v>000100</v>
+      </c>
+      <c r="F36">
+        <v>55</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h37</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
         <v>80</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>77</v>
       </c>
-      <c r="K37" t="s">
+      <c r="D37" s="14">
+        <v>48</v>
+      </c>
+      <c r="E37" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>110000</v>
+      </c>
+      <c r="F37">
+        <v>56</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h38</v>
+      </c>
+      <c r="I37" s="3">
+        <v>5</v>
+      </c>
+      <c r="L37" t="s">
         <v>84</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D38" s="14">
+        <v>8</v>
+      </c>
+      <c r="E38" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>001000</v>
+      </c>
+      <c r="F38">
+        <v>57</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h39</v>
+      </c>
+      <c r="I38" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>67</v>
       </c>
-      <c r="K39" t="s">
+      <c r="D39" s="14">
+        <v>45</v>
+      </c>
+      <c r="E39" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>101101</v>
+      </c>
+      <c r="F39">
+        <v>58</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h3A</v>
+      </c>
+      <c r="I39" s="3">
+        <v>34</v>
+      </c>
+      <c r="J39" t="s">
+        <v>32</v>
+      </c>
+      <c r="L39" t="s">
         <v>117</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>59</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h3B</v>
+      </c>
+      <c r="I40" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D41" s="14">
+        <v>16</v>
+      </c>
+      <c r="E41" s="23" t="str">
+        <f t="shared" ref="E41:E44" si="10">TEXT(DEC2BIN(D41),"000000")</f>
+        <v>010000</v>
+      </c>
+      <c r="F41">
+        <v>60</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h3C</v>
+      </c>
+      <c r="I41" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D42" s="14">
+        <v>52</v>
+      </c>
+      <c r="E42" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v>110100</v>
+      </c>
+      <c r="F42">
+        <v>61</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h3D</v>
+      </c>
+      <c r="I42" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D43" s="23">
+        <v>56</v>
+      </c>
+      <c r="E43" s="23" t="str">
+        <f t="shared" si="10"/>
+        <v>111000</v>
+      </c>
+      <c r="F43">
+        <v>62</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h3E</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>267</v>
+      </c>
+      <c r="D44" s="14">
+        <v>57</v>
+      </c>
+      <c r="E44" s="24" t="str">
+        <f t="shared" si="10"/>
+        <v>111001</v>
+      </c>
+      <c r="F44">
+        <v>63</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="7"/>
+        <v>8'h3F</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1892,7 +2418,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+      <c r="I47" s="17"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
@@ -1906,6 +2432,7 @@
       <c r="T47" s="5"/>
       <c r="U47" s="5"/>
       <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
@@ -1920,532 +2447,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A3:AB83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="29.44140625" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>205</v>
-      </c>
-      <c r="G1" t="s">
-        <v>141</v>
-      </c>
-      <c r="H1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" t="s">
-        <v>219</v>
-      </c>
-      <c r="H2" t="s">
-        <v>143</v>
-      </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>227</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="Q5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" t="s">
-        <v>204</v>
-      </c>
-      <c r="H7" t="s">
-        <v>146</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q7" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="R7" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E8" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" t="s">
-        <v>147</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q8" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="R8" s="15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>148</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q9" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>129</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="R10" s="15" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" t="s">
-        <v>159</v>
-      </c>
-      <c r="G11" t="s">
-        <v>149</v>
-      </c>
-      <c r="H11" t="s">
-        <v>150</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="N11" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q11" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="R11" s="15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" t="s">
-        <v>204</v>
-      </c>
-      <c r="H12" t="s">
-        <v>151</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q12" s="15">
-        <v>101</v>
-      </c>
-      <c r="R12" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" t="s">
-        <v>152</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="Q13" s="15">
-        <v>111</v>
-      </c>
-      <c r="R13" s="15" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>132</v>
-      </c>
-      <c r="M14" s="10"/>
-      <c r="N14" s="11"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>131</v>
-      </c>
-      <c r="D16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="N16" s="10">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" t="s">
-        <v>59</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="N17" s="10">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>133</v>
-      </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>138</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="N19" s="10">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" t="s">
-        <v>118</v>
-      </c>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>232</v>
-      </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>231</v>
-      </c>
-      <c r="B33" t="s">
-        <v>169</v>
-      </c>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I38" s="10"/>
-      <c r="J38" s="11"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J43" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="L5:N5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AB81"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2340" topLeftCell="A61" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="AB17" sqref="AB17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2340" topLeftCell="A74" activePane="bottomLeft"/>
+      <selection activeCell="U4" sqref="U4"/>
+      <selection pane="bottomLeft" activeCell="X77" sqref="X77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2464,87 +2471,87 @@
   <sheetData>
     <row r="3" spans="1:28" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
+      <c r="J3" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="V3" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y3" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="X3" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>243</v>
-      </c>
       <c r="AA3" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="AB3" s="13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="R4" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q4" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>156</v>
-      </c>
       <c r="S4" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
@@ -2556,13 +2563,13 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s">
         <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E5" s="14">
         <v>1</v>
@@ -2576,7 +2583,7 @@
         <v>1010</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J5" s="6">
         <v>0</v>
@@ -2636,10 +2643,10 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E6" s="14">
         <v>2</v>
@@ -2713,13 +2720,13 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
         <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E7" s="14">
         <v>3</v>
@@ -2733,7 +2740,7 @@
         <v>1010</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J7" s="6">
         <v>0</v>
@@ -2793,20 +2800,20 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>128</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E9" s="14">
         <v>4</v>
@@ -2880,10 +2887,10 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E10" s="14">
         <v>5</v>
@@ -2894,10 +2901,10 @@
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J10" s="6">
         <v>0</v>
@@ -2957,13 +2964,13 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E11" s="14">
         <v>6</v>
@@ -3037,10 +3044,10 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E12" s="14">
         <v>7</v>
@@ -3051,10 +3058,10 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J12" s="6">
         <v>0</v>
@@ -3114,17 +3121,17 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E14" s="14">
         <v>8</v>
@@ -3198,10 +3205,10 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E15" s="14">
         <v>9</v>
@@ -3212,10 +3219,10 @@
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J15" s="6">
         <v>0</v>
@@ -3275,13 +3282,13 @@
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
         <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E16" s="14">
         <v>10</v>
@@ -3295,7 +3302,7 @@
         <v>1001</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J16" s="6">
         <v>0</v>
@@ -3355,10 +3362,10 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E17" s="14">
         <v>11</v>
@@ -3432,7 +3439,7 @@
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
         <v>131</v>
@@ -3445,7 +3452,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E19" s="14">
         <v>12</v>
@@ -3522,7 +3529,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E20" s="14">
         <v>13</v>
@@ -3533,10 +3540,10 @@
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J20" s="6">
         <v>0</v>
@@ -3605,7 +3612,7 @@
         <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E22" s="14">
         <v>14</v>
@@ -3682,7 +3689,7 @@
         <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E23" s="14">
         <v>15</v>
@@ -3693,10 +3700,10 @@
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J23" s="6">
         <v>0</v>
@@ -3765,7 +3772,7 @@
         <v>123</v>
       </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E25" s="14">
         <v>16</v>
@@ -3842,7 +3849,7 @@
         <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E26" s="14">
         <v>17</v>
@@ -3853,10 +3860,10 @@
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J26" s="6">
         <v>0</v>
@@ -3925,7 +3932,7 @@
         <v>78</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E28" s="14">
         <v>18</v>
@@ -3936,10 +3943,10 @@
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J28" s="6">
         <v>0</v>
@@ -3998,13 +4005,13 @@
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E29" s="14">
         <v>19</v>
@@ -4078,13 +4085,13 @@
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E30" s="14">
         <v>20</v>
@@ -4095,10 +4102,10 @@
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J30" s="6">
         <v>0</v>
@@ -4158,7 +4165,7 @@
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -4168,13 +4175,13 @@
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
         <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E32" s="14">
         <v>21</v>
@@ -4185,10 +4192,10 @@
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J32" s="6">
         <v>0</v>
@@ -4247,13 +4254,13 @@
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D33" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E33" s="14">
         <v>22</v>
@@ -4327,13 +4334,13 @@
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B34" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E34" s="14">
         <v>23</v>
@@ -4344,10 +4351,10 @@
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J34" s="6">
         <v>0</v>
@@ -4411,7 +4418,7 @@
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E36" s="14">
         <v>24</v>
@@ -4422,10 +4429,10 @@
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I36" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J36" s="6">
         <v>0</v>
@@ -4484,7 +4491,7 @@
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E37" s="14">
         <v>25</v>
@@ -4558,7 +4565,7 @@
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E38" s="14">
         <v>26</v>
@@ -4569,10 +4576,10 @@
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J38" s="6">
         <v>0</v>
@@ -4636,7 +4643,7 @@
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E40" s="14">
         <v>27</v>
@@ -4647,10 +4654,10 @@
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J40" s="6">
         <v>0</v>
@@ -4709,7 +4716,7 @@
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E41" s="14">
         <v>28</v>
@@ -4723,7 +4730,7 @@
         <v>1001</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J41" s="6">
         <v>0</v>
@@ -4782,7 +4789,7 @@
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E42" s="14">
         <v>29</v>
@@ -4858,7 +4865,7 @@
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E44" s="14">
         <v>30</v>
@@ -4868,10 +4875,10 @@
         <v>011110</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J44" s="6">
         <v>0</v>
@@ -4930,7 +4937,7 @@
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E45" s="14">
         <v>31</v>
@@ -4943,7 +4950,7 @@
         <v>1001</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J45" s="6">
         <v>0</v>
@@ -5002,7 +5009,7 @@
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E46" s="14">
         <v>32</v>
@@ -5077,7 +5084,7 @@
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E48" s="14">
         <v>33</v>
@@ -5087,10 +5094,10 @@
         <v>100001</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J48" s="6">
         <v>0</v>
@@ -5149,7 +5156,7 @@
     </row>
     <row r="49" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E49" s="14">
         <v>34</v>
@@ -5162,7 +5169,7 @@
         <v>1001</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J49" s="6">
         <v>0</v>
@@ -5221,7 +5228,7 @@
     </row>
     <row r="50" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E50" s="14">
         <v>35</v>
@@ -5296,7 +5303,7 @@
     </row>
     <row r="52" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E52" s="14">
         <v>36</v>
@@ -5309,7 +5316,7 @@
         <v>1001</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J52" s="6">
         <v>0</v>
@@ -5368,7 +5375,7 @@
     </row>
     <row r="53" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E53" s="14">
         <v>37</v>
@@ -5381,7 +5388,7 @@
         <v>1001</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J53" s="6">
         <v>0</v>
@@ -5440,7 +5447,7 @@
     </row>
     <row r="54" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E54" s="14">
         <v>38</v>
@@ -5453,7 +5460,7 @@
         <v>1001</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J54" s="6">
         <v>0</v>
@@ -5515,7 +5522,7 @@
     </row>
     <row r="56" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E56" s="14">
         <v>39</v>
@@ -5525,10 +5532,10 @@
         <v>100111</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J56" s="6">
         <v>0</v>
@@ -5587,7 +5594,7 @@
     </row>
     <row r="57" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="E57" s="14">
         <v>40</v>
@@ -5597,10 +5604,10 @@
         <v>101000</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I57" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J57" s="6">
         <v>0</v>
@@ -5659,7 +5666,7 @@
     </row>
     <row r="58" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>137</v>
+        <v>47</v>
       </c>
       <c r="E58" s="14">
         <v>41</v>
@@ -5669,10 +5676,10 @@
         <v>101001</v>
       </c>
       <c r="H58" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J58" s="6">
         <v>0</v>
@@ -5963,10 +5970,10 @@
         <v>101101</v>
       </c>
       <c r="H64" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I64" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J64" s="6">
         <v>0</v>
@@ -6035,10 +6042,10 @@
         <v>101110</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I65" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J65" s="6">
         <v>0</v>
@@ -6107,10 +6114,10 @@
         <v>101111</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I66" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J66" s="6">
         <v>0</v>
@@ -6254,14 +6261,14 @@
         <v>49</v>
       </c>
       <c r="F70" s="7" t="str">
-        <f t="shared" ref="F70:F81" si="1">TEXT(DEC2BIN(E70),"000000")</f>
+        <f t="shared" ref="F70:F83" si="1">TEXT(DEC2BIN(E70),"000000")</f>
         <v>110001</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I70" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J70" s="6">
         <v>0</v>
@@ -6330,10 +6337,10 @@
         <v>110010</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I71" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J71" s="6">
         <v>0</v>
@@ -6402,10 +6409,10 @@
         <v>110011</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I72" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J72" s="6">
         <v>0</v>
@@ -6467,7 +6474,7 @@
     </row>
     <row r="74" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E74" s="14">
         <v>52</v>
@@ -6540,7 +6547,7 @@
     </row>
     <row r="75" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E75" s="7">
         <v>53</v>
@@ -6550,10 +6557,10 @@
         <v>110101</v>
       </c>
       <c r="H75" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I75" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J75" s="6">
         <v>1</v>
@@ -6615,7 +6622,7 @@
     </row>
     <row r="77" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E77" s="7">
         <v>54</v>
@@ -6690,7 +6697,7 @@
     </row>
     <row r="79" spans="4:28" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E79" s="7">
         <v>55</v>
@@ -6835,9 +6842,616 @@
         <v>0</v>
       </c>
     </row>
+    <row r="83" spans="4:28" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>267</v>
+      </c>
+      <c r="E83" s="7">
+        <v>57</v>
+      </c>
+      <c r="F83" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>111001</v>
+      </c>
+      <c r="H83" s="6">
+        <v>1111</v>
+      </c>
+      <c r="I83" s="6">
+        <v>110</v>
+      </c>
+      <c r="J83" s="24">
+        <v>0</v>
+      </c>
+      <c r="K83" s="24">
+        <v>0</v>
+      </c>
+      <c r="L83" s="24">
+        <v>0</v>
+      </c>
+      <c r="M83" s="24">
+        <v>0</v>
+      </c>
+      <c r="N83" s="24">
+        <v>0</v>
+      </c>
+      <c r="O83" s="24">
+        <v>0</v>
+      </c>
+      <c r="P83" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q83" s="24">
+        <v>0</v>
+      </c>
+      <c r="R83" s="24">
+        <v>0</v>
+      </c>
+      <c r="S83" s="24">
+        <v>0</v>
+      </c>
+      <c r="U83" s="24">
+        <v>0</v>
+      </c>
+      <c r="V83" s="24">
+        <v>0</v>
+      </c>
+      <c r="W83" s="24">
+        <v>0</v>
+      </c>
+      <c r="X83" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y83" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA83" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J3:S3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="H2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="Q5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H7" t="s">
+        <v>143</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" t="s">
+        <v>144</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H11" t="s">
+        <v>147</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" t="s">
+        <v>148</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q12" s="15">
+        <v>101</v>
+      </c>
+      <c r="R12" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" t="s">
+        <v>149</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>110</v>
+      </c>
+      <c r="R13" s="24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="Q14" s="15">
+        <v>111</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="N16" s="10">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="N17" s="10">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>133</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>135</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="N19" s="10">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>229</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>263</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B33" t="s">
+        <v>166</v>
+      </c>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I38" s="10"/>
+      <c r="J38" s="11"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="G32:I32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tested for some matrices
</commit_message>
<xml_diff>
--- a/Processor.xlsx
+++ b/Processor.xlsx
@@ -8,9 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="285">
   <si>
     <t>RA &lt;== T</t>
   </si>
@@ -1020,7 +1022,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1100,6 +1102,12 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1393,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="102" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="102" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1782,10 +1790,10 @@
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D14" s="14">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="22"/>
       <c r="I14" s="3" t="s">
@@ -2162,7 +2170,7 @@
         <v>62</v>
       </c>
       <c r="G33" t="str">
-        <f>"8'h"&amp;DEC2HEX(F33, 2)</f>
+        <f t="shared" ref="G33:G61" si="1">"8'h"&amp;DEC2HEX(F33, 2)</f>
         <v>8'h3E</v>
       </c>
       <c r="I33" s="3">
@@ -2184,7 +2192,7 @@
         <v>63</v>
       </c>
       <c r="G34" t="str">
-        <f>"8'h"&amp;DEC2HEX(F34, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h3F</v>
       </c>
       <c r="I34" s="3">
@@ -2211,7 +2219,7 @@
         <v>64</v>
       </c>
       <c r="G35" t="str">
-        <f>"8'h"&amp;DEC2HEX(F35, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h40</v>
       </c>
       <c r="I35" s="3">
@@ -2239,7 +2247,7 @@
         <v>65</v>
       </c>
       <c r="G36" t="str">
-        <f>"8'h"&amp;DEC2HEX(F36, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h41</v>
       </c>
       <c r="I36" s="3">
@@ -2264,7 +2272,7 @@
         <v>66</v>
       </c>
       <c r="G37" t="str">
-        <f>"8'h"&amp;DEC2HEX(F37, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h42</v>
       </c>
       <c r="I37" s="3">
@@ -2277,7 +2285,7 @@
         <v>67</v>
       </c>
       <c r="G38" t="str">
-        <f>"8'h"&amp;DEC2HEX(F38, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h43</v>
       </c>
       <c r="I38" s="3">
@@ -2302,7 +2310,7 @@
         <v>68</v>
       </c>
       <c r="G39" t="str">
-        <f>"8'h"&amp;DEC2HEX(F39, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h44</v>
       </c>
       <c r="I39" s="3">
@@ -2326,7 +2334,7 @@
         <v>69</v>
       </c>
       <c r="G40" t="str">
-        <f>"8'h"&amp;DEC2HEX(F40, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h45</v>
       </c>
       <c r="I40" s="3">
@@ -2345,7 +2353,7 @@
         <v>70</v>
       </c>
       <c r="G41" t="str">
-        <f>"8'h"&amp;DEC2HEX(F41, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h46</v>
       </c>
       <c r="I41" s="3">
@@ -2364,7 +2372,7 @@
         <v>71</v>
       </c>
       <c r="G42" t="str">
-        <f>"8'h"&amp;DEC2HEX(F42, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h47</v>
       </c>
       <c r="I42" s="3">
@@ -2389,7 +2397,7 @@
         <v>72</v>
       </c>
       <c r="G43" t="str">
-        <f>"8'h"&amp;DEC2HEX(F43, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h48</v>
       </c>
       <c r="I43" s="3">
@@ -2402,7 +2410,7 @@
         <v>73</v>
       </c>
       <c r="G44" t="str">
-        <f>"8'h"&amp;DEC2HEX(F44, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h49</v>
       </c>
       <c r="I44" s="3">
@@ -2423,7 +2431,7 @@
         <v>74</v>
       </c>
       <c r="G45" t="str">
-        <f>"8'h"&amp;DEC2HEX(F45, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h4A</v>
       </c>
       <c r="I45" s="3">
@@ -2441,7 +2449,7 @@
         <v>75</v>
       </c>
       <c r="G46" t="str">
-        <f>"8'h"&amp;DEC2HEX(F46, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h4B</v>
       </c>
       <c r="I46" s="3">
@@ -2459,7 +2467,7 @@
         <v>76</v>
       </c>
       <c r="G47" t="str">
-        <f>"8'h"&amp;DEC2HEX(F47, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h4C</v>
       </c>
       <c r="I47" s="3">
@@ -2477,7 +2485,7 @@
         <v>77</v>
       </c>
       <c r="G48" t="str">
-        <f>"8'h"&amp;DEC2HEX(F48, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h4D</v>
       </c>
       <c r="I48" s="3">
@@ -2489,7 +2497,7 @@
         <v>78</v>
       </c>
       <c r="G49" t="str">
-        <f>"8'h"&amp;DEC2HEX(F49, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h4E</v>
       </c>
       <c r="I49" s="3">
@@ -2507,7 +2515,7 @@
         <v>79</v>
       </c>
       <c r="G50" t="str">
-        <f>"8'h"&amp;DEC2HEX(F50, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h4F</v>
       </c>
       <c r="I50" s="3">
@@ -2525,7 +2533,7 @@
         <v>80</v>
       </c>
       <c r="G51" t="str">
-        <f>"8'h"&amp;DEC2HEX(F51, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h50</v>
       </c>
       <c r="I51" s="3">
@@ -2543,7 +2551,7 @@
         <v>81</v>
       </c>
       <c r="G52" t="str">
-        <f>"8'h"&amp;DEC2HEX(F52, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h51</v>
       </c>
       <c r="I52" s="3">
@@ -2561,7 +2569,7 @@
         <v>82</v>
       </c>
       <c r="G53" t="str">
-        <f>"8'h"&amp;DEC2HEX(F53, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h52</v>
       </c>
       <c r="I53" s="3">
@@ -2572,17 +2580,11 @@
       </c>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>265</v>
-      </c>
-      <c r="D54" s="14">
-        <v>57</v>
-      </c>
       <c r="F54">
         <v>83</v>
       </c>
       <c r="G54" t="str">
-        <f>"8'h"&amp;DEC2HEX(F54, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h53</v>
       </c>
       <c r="I54" s="3">
@@ -2590,11 +2592,17 @@
       </c>
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="30">
+        <v>55</v>
+      </c>
       <c r="F55">
         <v>84</v>
       </c>
       <c r="G55" t="str">
-        <f>"8'h"&amp;DEC2HEX(F55, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h54</v>
       </c>
       <c r="I55" s="3">
@@ -2602,11 +2610,17 @@
       </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="14">
+        <v>8</v>
+      </c>
       <c r="F56">
         <v>85</v>
       </c>
       <c r="G56" t="str">
-        <f>"8'h"&amp;DEC2HEX(F56, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h55</v>
       </c>
       <c r="I56" s="3">
@@ -2618,7 +2632,7 @@
         <v>86</v>
       </c>
       <c r="G57" t="str">
-        <f>"8'h"&amp;DEC2HEX(F57, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h56</v>
       </c>
       <c r="I57" s="3">
@@ -2626,11 +2640,17 @@
       </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>265</v>
+      </c>
+      <c r="D58" s="14">
+        <v>57</v>
+      </c>
       <c r="F58">
         <v>87</v>
       </c>
       <c r="G58" t="str">
-        <f>"8'h"&amp;DEC2HEX(F58, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h57</v>
       </c>
       <c r="I58" s="3">
@@ -2642,7 +2662,7 @@
         <v>88</v>
       </c>
       <c r="G59" t="str">
-        <f>"8'h"&amp;DEC2HEX(F59, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h58</v>
       </c>
       <c r="I59" s="3">
@@ -2654,7 +2674,7 @@
         <v>89</v>
       </c>
       <c r="G60" t="str">
-        <f>"8'h"&amp;DEC2HEX(F60, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h59</v>
       </c>
       <c r="I60" s="3">
@@ -2666,7 +2686,7 @@
         <v>90</v>
       </c>
       <c r="G61" t="str">
-        <f>"8'h"&amp;DEC2HEX(F61, 2)</f>
+        <f t="shared" si="1"/>
         <v>8'h5A</v>
       </c>
       <c r="I61" s="3">
@@ -2681,10 +2701,1465 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="10" width="8.88671875" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="17">
+        <v>23</v>
+      </c>
+      <c r="C2" s="18">
+        <v>45</v>
+      </c>
+      <c r="D2" s="18">
+        <v>44</v>
+      </c>
+      <c r="E2" s="20">
+        <v>56</v>
+      </c>
+      <c r="G2" s="17">
+        <v>66</v>
+      </c>
+      <c r="H2" s="18">
+        <v>12</v>
+      </c>
+      <c r="I2" s="18">
+        <v>55</v>
+      </c>
+      <c r="J2" s="20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="17">
+        <v>66</v>
+      </c>
+      <c r="C3" s="18">
+        <v>77</v>
+      </c>
+      <c r="D3" s="18">
+        <v>3</v>
+      </c>
+      <c r="E3" s="20">
+        <v>45</v>
+      </c>
+      <c r="G3" s="17">
+        <v>34</v>
+      </c>
+      <c r="H3" s="18">
+        <v>43</v>
+      </c>
+      <c r="I3" s="18">
+        <v>4</v>
+      </c>
+      <c r="J3" s="20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="17">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18">
+        <v>32</v>
+      </c>
+      <c r="D4" s="18">
+        <v>34</v>
+      </c>
+      <c r="E4" s="20">
+        <v>53</v>
+      </c>
+      <c r="G4" s="17">
+        <v>56</v>
+      </c>
+      <c r="H4" s="18">
+        <v>67</v>
+      </c>
+      <c r="I4" s="18">
+        <v>5</v>
+      </c>
+      <c r="J4" s="20">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="17">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18">
+        <v>56</v>
+      </c>
+      <c r="D5" s="18">
+        <v>12</v>
+      </c>
+      <c r="E5" s="20">
+        <v>23</v>
+      </c>
+      <c r="G5" s="17">
+        <v>98</v>
+      </c>
+      <c r="H5" s="18">
+        <v>91</v>
+      </c>
+      <c r="I5" s="18">
+        <v>90</v>
+      </c>
+      <c r="J5" s="20">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>60</v>
+      </c>
+      <c r="C9" t="str">
+        <f>"8'h"&amp;DEC2HEX(B9, 2)</f>
+        <v>8'h3C</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>61</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" ref="C10:C60" si="0">"8'h"&amp;DEC2HEX(B10, 2)</f>
+        <v>8'h3D</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>62</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h3E</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11" s="3">
+        <v>4</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>63</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h3F</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>64</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h40</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13" s="3">
+        <v>23</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>65</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h41</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>66</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h42</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>67</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h43</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>68</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h44</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>69</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h45</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>70</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h46</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>71</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h47</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>72</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h48</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>73</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h49</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>74</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4A</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>75</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4B</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>76</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4C</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>77</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4D</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>78</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4E</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>79</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4F</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>80</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h50</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" s="3">
+        <v>66</v>
+      </c>
+      <c r="F29" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>81</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h51</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>82</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h52</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31" s="3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>83</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h53</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>84</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h54</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>85</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h55</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>86</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h56</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>87</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h57</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>88</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h58</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>89</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h59</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>90</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5A</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>91</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5B</v>
+      </c>
+      <c r="E40" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>92</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5C</v>
+      </c>
+      <c r="E41" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>93</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5D</v>
+      </c>
+      <c r="E42" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>94</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5E</v>
+      </c>
+      <c r="E43" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>95</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5F</v>
+      </c>
+      <c r="E44" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>96</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h60</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
+      <c r="F45" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>97</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h61</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>98</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h62</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>99</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h63</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>100</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h64</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>101</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h65</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>102</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h66</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>103</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h67</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>104</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h68</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>105</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h69</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>106</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h6A</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>107</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h6B</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>108</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h6C</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>109</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h6D</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>110</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h6E</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>111</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h6F</v>
+      </c>
+      <c r="E60" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="9" width="8.88671875" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="17">
+        <v>34</v>
+      </c>
+      <c r="C2" s="18">
+        <v>44</v>
+      </c>
+      <c r="D2" s="18">
+        <v>71</v>
+      </c>
+      <c r="E2" s="20">
+        <v>43</v>
+      </c>
+      <c r="G2" s="17">
+        <v>66</v>
+      </c>
+      <c r="H2" s="18">
+        <v>12</v>
+      </c>
+      <c r="I2" s="20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="17">
+        <v>12</v>
+      </c>
+      <c r="C3" s="18">
+        <v>78</v>
+      </c>
+      <c r="D3" s="18">
+        <v>55</v>
+      </c>
+      <c r="E3" s="20">
+        <v>92</v>
+      </c>
+      <c r="G3" s="17">
+        <v>34</v>
+      </c>
+      <c r="H3" s="18">
+        <v>43</v>
+      </c>
+      <c r="I3" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+      <c r="C4" s="31">
+        <v>1</v>
+      </c>
+      <c r="D4" s="31">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+      <c r="G4" s="17">
+        <v>56</v>
+      </c>
+      <c r="H4" s="18">
+        <v>67</v>
+      </c>
+      <c r="I4" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="17">
+        <v>98</v>
+      </c>
+      <c r="H5" s="18">
+        <v>91</v>
+      </c>
+      <c r="I5" s="20">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8" t="str">
+        <f>"8'h"&amp;DEC2HEX(B8, 2)</f>
+        <v>8'h3C</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>61</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ref="C9:C41" si="0">"8'h"&amp;DEC2HEX(B9, 2)</f>
+        <v>8'h3D</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>62</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h3E</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10" s="3">
+        <v>4</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>63</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h3F</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11" s="3">
+        <v>3</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>64</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h40</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12" s="3">
+        <v>34</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>65</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h41</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>66</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h42</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>67</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h43</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>68</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h44</v>
+      </c>
+      <c r="D16"/>
+      <c r="E16" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>69</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h45</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>70</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h46</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>71</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h47</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>72</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h48</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>73</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h49</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>74</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4A</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>75</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4B</v>
+      </c>
+      <c r="D23"/>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>76</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4C</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" s="3">
+        <v>66</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>77</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4D</v>
+      </c>
+      <c r="D25"/>
+      <c r="E25" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>78</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4E</v>
+      </c>
+      <c r="D26"/>
+      <c r="E26" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>79</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h4F</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>80</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h50</v>
+      </c>
+      <c r="D28"/>
+      <c r="E28" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>81</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h51</v>
+      </c>
+      <c r="D29"/>
+      <c r="E29" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>82</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h52</v>
+      </c>
+      <c r="D30"/>
+      <c r="E30" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>83</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h53</v>
+      </c>
+      <c r="D31"/>
+      <c r="E31" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>84</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h54</v>
+      </c>
+      <c r="D32"/>
+      <c r="E32" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>85</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h55</v>
+      </c>
+      <c r="D33"/>
+      <c r="E33" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>86</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h56</v>
+      </c>
+      <c r="D34"/>
+      <c r="E34" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>87</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h57</v>
+      </c>
+      <c r="D35"/>
+      <c r="E35" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>88</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h58</v>
+      </c>
+      <c r="D36"/>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>89</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h59</v>
+      </c>
+      <c r="D37"/>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>90</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5A</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>91</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5B</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>92</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5C</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>93</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>8'h5D</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>94</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" ref="C42:C44" si="1">"8'h"&amp;DEC2HEX(B42, 2)</f>
+        <v>8'h5E</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>95</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="1"/>
+        <v>8'h5F</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>96</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="1"/>
+        <v>8'h60</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="E45"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="E46"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="E47"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48"/>
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49"/>
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50"/>
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51"/>
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52"/>
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53"/>
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54"/>
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55"/>
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56"/>
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57"/>
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58"/>
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59"/>
+      <c r="C59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2725,14 +4200,14 @@
       <c r="H2" t="s">
         <v>138</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
@@ -2757,11 +4232,11 @@
       <c r="B5" t="s">
         <v>222</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
       <c r="Q5" t="s">
         <v>231</v>
       </c>
@@ -3141,8 +4616,8 @@
       <c r="E29" t="s">
         <v>116</v>
       </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -3163,11 +4638,11 @@
       <c r="F32" t="s">
         <v>261</v>
       </c>
-      <c r="G32" s="30" t="s">
+      <c r="G32" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
       <c r="J32" s="10"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -3230,14 +4705,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AC87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2340" topLeftCell="A51" activePane="bottomLeft"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2340" topLeftCell="A46" activePane="bottomLeft"/>
       <selection activeCell="J4" sqref="J4"/>
-      <selection pane="bottomLeft" activeCell="P57" sqref="P57"/>
+      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3268,19 +4743,19 @@
       <c r="I3" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
-      <c r="T3" s="32"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
       <c r="U3" s="8"/>
       <c r="V3" s="8" t="s">
         <v>239</v>
@@ -8049,7 +9524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>